<commit_message>
changing calibration_reports_measure to CalibrationReportsMeasure in the outputs tab
</commit_message>
<xml_diff>
--- a/projects/SEB_Diag_2013.xlsx
+++ b/projects/SEB_Diag_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2184,42 +2184,6 @@
     <t>CalibrationReportsEnhanced20</t>
   </si>
   <si>
-    <t>calibration_reports_enhanced20.gas_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_nmbe_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_nmbe_within_limit</t>
-  </si>
-  <si>
     <t>SEB4 baseboard Diag 2013</t>
   </si>
   <si>
@@ -2257,6 +2221,42 @@
   </si>
   <si>
     <t>Run Measure 2</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_modeled</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_modeled</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_rmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_rmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_nmbe_within_limit</t>
   </si>
 </sst>
 </file>
@@ -6680,7 +6680,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>726</v>
+        <v>714</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>467</v>
@@ -6748,7 +6748,7 @@
         <v>449</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>727</v>
+        <v>715</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -6774,13 +6774,13 @@
     </row>
     <row r="22" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>729</v>
+        <v>717</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>729</v>
+        <v>717</v>
       </c>
       <c r="D22" s="33"/>
     </row>
@@ -6951,7 +6951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
@@ -7499,10 +7499,10 @@
         <v>283</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>733</v>
+        <v>721</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>733</v>
+        <v>721</v>
       </c>
       <c r="E24" s="39" t="s">
         <v>66</v>
@@ -7513,10 +7513,10 @@
         <v>22</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>737</v>
+        <v>725</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>730</v>
+        <v>718</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>63</v>
@@ -7537,11 +7537,11 @@
         <v>1</v>
       </c>
       <c r="P25" s="37" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
       <c r="Q25" s="38"/>
       <c r="R25" s="37" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -7757,10 +7757,10 @@
         <v>666</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>734</v>
+        <v>722</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>734</v>
+        <v>722</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>66</v>
@@ -7771,10 +7771,10 @@
         <v>22</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>738</v>
+        <v>726</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>730</v>
+        <v>718</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>63</v>
@@ -7795,11 +7795,11 @@
         <v>1</v>
       </c>
       <c r="P36" s="37" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
       <c r="Q36" s="38"/>
       <c r="R36" s="37" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8033,10 +8033,10 @@
         <v>671</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>735</v>
+        <v>723</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>735</v>
+        <v>723</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>66</v>
@@ -8047,10 +8047,10 @@
         <v>22</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>736</v>
+        <v>724</v>
       </c>
       <c r="E48" s="37" t="s">
-        <v>730</v>
+        <v>718</v>
       </c>
       <c r="G48" s="37" t="s">
         <v>63</v>
@@ -8071,11 +8071,11 @@
         <v>1</v>
       </c>
       <c r="P48" s="37" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
       <c r="Q48" s="38"/>
       <c r="R48" s="37" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
@@ -8590,9 +8590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD25"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8739,7 +8739,7 @@
       <c r="B5" s="40"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>634</v>
@@ -8768,7 +8768,7 @@
       <c r="B6" s="40"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29" t="s">
-        <v>714</v>
+        <v>728</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>636</v>
@@ -8797,7 +8797,7 @@
       <c r="B7" s="40"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>641</v>
@@ -8825,7 +8825,7 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>715</v>
+        <v>730</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>641</v>
@@ -8853,7 +8853,7 @@
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>641</v>
@@ -8881,7 +8881,7 @@
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>641</v>
@@ -8909,7 +8909,7 @@
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>716</v>
+        <v>733</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>641</v>
@@ -8937,7 +8937,7 @@
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>717</v>
+        <v>734</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>641</v>
@@ -8965,7 +8965,7 @@
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>724</v>
+        <v>735</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="30" t="s">
@@ -8988,7 +8988,7 @@
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>725</v>
+        <v>736</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="30" t="s">
@@ -9011,7 +9011,7 @@
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>718</v>
+        <v>737</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="30" t="s">
@@ -9033,7 +9033,7 @@
       </c>
       <c r="B16" s="29"/>
       <c r="D16" s="29" t="s">
-        <v>719</v>
+        <v>738</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
true up algorithm params
</commit_message>
<xml_diff>
--- a/projects/SEB_Diag_2013.xlsx
+++ b/projects/SEB_Diag_2013.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="743">
   <si>
     <t>type</t>
   </si>
@@ -2263,6 +2263,12 @@
   </si>
   <si>
     <t xml:space="preserve">1 or 0 </t>
+  </si>
+  <si>
+    <t>Failed F Value</t>
+  </si>
+  <si>
+    <t>Debug Messages</t>
   </si>
 </sst>
 </file>
@@ -4292,7 +4298,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4392,7 +4398,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1851">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6547,7 +6552,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6816,13 +6821,25 @@
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28"/>
+      <c r="A25" s="30" t="s">
+        <v>741</v>
+      </c>
+      <c r="B25" s="28">
+        <v>1E+18</v>
+      </c>
       <c r="C25" s="29"/>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="28"/>
-      <c r="C26" s="53"/>
+      <c r="A26" s="30" t="s">
+        <v>742</v>
+      </c>
+      <c r="B26" s="29">
+        <v>0</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>740</v>
+      </c>
       <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update spreadsheets to enforce measure order by type
</commit_message>
<xml_diff>
--- a/projects/SEB_Diag_2013.xlsx
+++ b/projects/SEB_Diag_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$73</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -6554,7 +6554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -6985,11 +6985,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z147"/>
+  <dimension ref="A1:Z146"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7508,150 +7508,152 @@
       </c>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="b">
+    <row r="23" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="35" t="s">
-        <v>710</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>713</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>713</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>231</v>
-      </c>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-    </row>
-    <row r="24" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="b">
+      <c r="B23" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>721</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>721</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>725</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>718</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="37">
         <v>1</v>
       </c>
-      <c r="B24" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>721</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>721</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>725</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>718</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="37">
+      <c r="K24" s="37">
+        <v>0</v>
+      </c>
+      <c r="L24" s="37">
         <v>1</v>
       </c>
-      <c r="K25" s="37">
-        <v>0</v>
-      </c>
-      <c r="L25" s="37">
+      <c r="M24" s="37">
         <v>1</v>
       </c>
-      <c r="M25" s="37">
+      <c r="N24" s="37">
         <v>1</v>
       </c>
-      <c r="N25" s="37">
+      <c r="P24" s="37" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="37" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="50"/>
+      <c r="G25" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>640</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26" s="50"/>
+      <c r="G26" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="I26" s="30">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>-80</v>
+      </c>
+      <c r="L26" s="3">
+        <v>80</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
+        <f>(L26-K26)/6</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="O26" s="3">
         <v>1</v>
       </c>
-      <c r="P25" s="37" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="37" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>371</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>640</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>286</v>
+      <c r="R26" s="30" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="F27" s="50"/>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="29" t="s">
         <v>641</v>
       </c>
-      <c r="I27" s="30">
-        <v>0</v>
-      </c>
-      <c r="K27" s="3">
-        <v>-80</v>
-      </c>
-      <c r="L27" s="3">
-        <v>80</v>
-      </c>
-      <c r="M27" s="3">
-        <v>0</v>
-      </c>
-      <c r="N27" s="3">
-        <f>(L27-K27)/6</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="O27" s="3">
-        <v>1</v>
-      </c>
-      <c r="R27" s="30" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I27" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="50"/>
+        <v>48</v>
+      </c>
+      <c r="F28" s="49"/>
       <c r="G28" s="29" t="s">
         <v>62</v>
       </c>
@@ -7667,17 +7669,17 @@
         <v>21</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F29" s="49"/>
       <c r="G29" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="I29" s="29">
         <v>0</v>
@@ -7688,19 +7690,16 @@
         <v>21</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F30" s="49"/>
       <c r="G30" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>645</v>
-      </c>
-      <c r="I30" s="29">
+        <v>61</v>
+      </c>
+      <c r="I30" s="29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7709,17 +7708,20 @@
         <v>21</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F31" s="49"/>
       <c r="G31" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="29" t="b">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>645</v>
+      </c>
+      <c r="I31" s="29">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7727,176 +7729,173 @@
         <v>21</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F32" s="49"/>
       <c r="G32" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>641</v>
+      </c>
+      <c r="I32" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B33" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>649</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="50"/>
+      <c r="G33" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="29" t="s">
+      <c r="H33" s="29" t="s">
         <v>645</v>
       </c>
-      <c r="I32" s="29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>648</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="29" t="s">
+      <c r="I33" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>666</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>722</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>722</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>726</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>718</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="37">
+        <v>1</v>
+      </c>
+      <c r="K35" s="37">
+        <v>0</v>
+      </c>
+      <c r="L35" s="37">
+        <v>1</v>
+      </c>
+      <c r="M35" s="37">
+        <v>1</v>
+      </c>
+      <c r="N35" s="37">
+        <v>1</v>
+      </c>
+      <c r="P35" s="37" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="37" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="50"/>
+      <c r="G36" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>668</v>
+      </c>
+      <c r="F37" s="50"/>
+      <c r="G37" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="29" t="s">
+      <c r="H37" s="30" t="s">
         <v>641</v>
       </c>
-      <c r="I33" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>649</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="50"/>
-      <c r="G34" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>645</v>
-      </c>
-      <c r="I34" s="29">
+      <c r="I37" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N37" s="3">
+        <f>(L37-K37)/6</f>
+        <v>3.3333333333333326E-2</v>
+      </c>
+      <c r="O37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>666</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>722</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>722</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>726</v>
-      </c>
-      <c r="E36" s="37" t="s">
-        <v>718</v>
-      </c>
-      <c r="G36" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" s="37">
-        <v>1</v>
-      </c>
-      <c r="K36" s="37">
-        <v>0</v>
-      </c>
-      <c r="L36" s="37">
-        <v>1</v>
-      </c>
-      <c r="M36" s="37">
-        <v>1</v>
-      </c>
-      <c r="N36" s="37">
-        <v>1</v>
-      </c>
-      <c r="P36" s="37" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q36" s="38"/>
-      <c r="R36" s="37" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B37" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>342</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="50"/>
-      <c r="G37" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="I37" s="42" t="s">
-        <v>415</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B38" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>667</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>668</v>
-      </c>
-      <c r="F38" s="50"/>
-      <c r="G38" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="30" t="s">
-        <v>641</v>
-      </c>
-      <c r="I38" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0.78</v>
-      </c>
-      <c r="L38" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="M38" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="N38" s="3">
-        <f>(L38-K38)/6</f>
-        <v>3.3333333333333326E-2</v>
-      </c>
-      <c r="O38" s="3">
-        <v>1</v>
-      </c>
-      <c r="R38" s="30" t="s">
+      <c r="R37" s="30" t="s">
         <v>711</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="30"/>
+      <c r="G38" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="I38" s="29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7904,16 +7903,19 @@
         <v>21</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>347</v>
+        <v>642</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="F39" s="30"/>
       <c r="G39" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="I39" s="29" t="b">
+        <v>62</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>641</v>
+      </c>
+      <c r="I39" s="29">
         <v>0</v>
       </c>
     </row>
@@ -7922,10 +7924,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="F40" s="30"/>
       <c r="G40" s="29" t="s">
@@ -7943,40 +7945,37 @@
         <v>21</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="I41" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="30"/>
+        <v>52</v>
+      </c>
+      <c r="F42" s="50"/>
       <c r="G42" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>645</v>
-      </c>
-      <c r="I42" s="29">
+        <v>61</v>
+      </c>
+      <c r="I42" s="29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7985,17 +7984,20 @@
         <v>21</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F43" s="50"/>
       <c r="G43" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="I43" s="29" t="b">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>645</v>
+      </c>
+      <c r="I43" s="29">
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8003,20 +8005,20 @@
         <v>21</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F44" s="50"/>
       <c r="G44" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="I44" s="29">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8024,196 +8026,179 @@
         <v>21</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F45" s="50"/>
       <c r="G45" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>645</v>
+      </c>
+      <c r="I45" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="39" t="s">
+        <v>671</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>723</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>723</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>724</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>718</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="37">
+        <v>1</v>
+      </c>
+      <c r="K47" s="37">
+        <v>0</v>
+      </c>
+      <c r="L47" s="37">
+        <v>1</v>
+      </c>
+      <c r="M47" s="37">
+        <v>1</v>
+      </c>
+      <c r="N47" s="37">
+        <v>1</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="37" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>674</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>672</v>
+      </c>
+      <c r="F48" s="49"/>
+      <c r="G48" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="H48" s="43" t="s">
         <v>641</v>
       </c>
-      <c r="I45" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>649</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="F46" s="50"/>
-      <c r="G46" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="29" t="s">
-        <v>645</v>
-      </c>
-      <c r="I46" s="29">
+      <c r="I48" s="43">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="39" t="b">
+      <c r="J48" s="45"/>
+      <c r="K48" s="44">
+        <v>0.9</v>
+      </c>
+      <c r="L48" s="44">
         <v>1</v>
       </c>
-      <c r="B47" s="39" t="s">
-        <v>671</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>723</v>
-      </c>
-      <c r="D47" s="39" t="s">
-        <v>723</v>
-      </c>
-      <c r="E47" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="37" t="s">
-        <v>724</v>
-      </c>
-      <c r="E48" s="37" t="s">
-        <v>718</v>
-      </c>
-      <c r="G48" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="I48" s="37">
+      <c r="M48" s="44">
+        <v>0.95</v>
+      </c>
+      <c r="N48" s="44">
+        <f>(L48-K48)/6</f>
+        <v>1.6666666666666663E-2</v>
+      </c>
+      <c r="O48" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="R48" s="37" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>675</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="F49" s="50"/>
+      <c r="G49" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="I49" s="30">
+        <v>1450</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <v>3000</v>
+      </c>
+      <c r="M49" s="3">
+        <v>1450</v>
+      </c>
+      <c r="N49" s="3">
+        <f>(L49-K49)/6</f>
+        <v>500</v>
+      </c>
+      <c r="O49" s="3">
+        <v>10</v>
+      </c>
+      <c r="R49" s="30" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="K48" s="37">
-        <v>0</v>
-      </c>
-      <c r="L48" s="37">
-        <v>1</v>
-      </c>
-      <c r="M48" s="37">
-        <v>1</v>
-      </c>
-      <c r="N48" s="37">
-        <v>1</v>
-      </c>
-      <c r="P48" s="37" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q48" s="38"/>
-      <c r="R48" s="37" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="43" t="s">
-        <v>674</v>
-      </c>
-      <c r="E49" s="43" t="s">
-        <v>672</v>
-      </c>
-      <c r="F49" s="49"/>
-      <c r="G49" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="H49" s="43" t="s">
-        <v>641</v>
-      </c>
-      <c r="I49" s="43">
-        <v>1</v>
-      </c>
-      <c r="J49" s="45"/>
-      <c r="K49" s="44">
-        <v>0.9</v>
-      </c>
-      <c r="L49" s="44">
-        <v>1</v>
-      </c>
-      <c r="M49" s="44">
-        <v>0.95</v>
-      </c>
-      <c r="N49" s="44">
-        <f>(L49-K49)/6</f>
-        <v>1.6666666666666663E-2</v>
-      </c>
-      <c r="O49" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="R49" s="37" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="30" t="s">
-        <v>675</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="F50" s="50"/>
-      <c r="G50" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H50" s="30" t="s">
-        <v>641</v>
-      </c>
-      <c r="I50" s="30">
-        <v>1450</v>
-      </c>
-      <c r="K50" s="3">
-        <v>0</v>
-      </c>
-      <c r="L50" s="3">
-        <v>3000</v>
-      </c>
-      <c r="M50" s="3">
-        <v>1450</v>
-      </c>
-      <c r="N50" s="3">
-        <f>(L50-K50)/6</f>
-        <v>500</v>
-      </c>
-      <c r="O50" s="3">
-        <v>10</v>
-      </c>
-      <c r="R50" s="30" t="s">
-        <v>711</v>
-      </c>
+      <c r="B50" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>713</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>713</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="35"/>
-      <c r="P51" s="35"/>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
+      <c r="F51" s="40"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F52" s="40"/>
@@ -8251,7 +8236,6 @@
       <c r="J58" s="30"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F59" s="40"/>
       <c r="I59" s="30"/>
       <c r="J59" s="30"/>
     </row>
@@ -8603,12 +8587,8 @@
       <c r="I146" s="30"/>
       <c r="J146" s="30"/>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I147" s="30"/>
-      <c r="J147" s="30"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:AA74"/>
+  <autoFilter ref="A2:AA73"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>

</xml_diff>